<commit_message>
Finished User Story for Admin, Newsagent and Delivery Doc
</commit_message>
<xml_diff>
--- a/User Stories/DeliveryUserStory.xlsx
+++ b/User Stories/DeliveryUserStory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronan\OneDrive\Documents\GitHub\Newsagent-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14439FCE-C5CD-4B86-A903-60C3B147CFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC537A-D0F5-44B4-B8C1-590AB52AA478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,16 +508,16 @@
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.1796875" customWidth="1"/>
-    <col min="5" max="5" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.19921875" customWidth="1"/>
+    <col min="5" max="5" width="52.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -530,7 +530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -543,7 +543,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -560,7 +560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -568,7 +568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -576,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -599,12 +599,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>18</v>
       </c>
@@ -612,7 +612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -620,12 +620,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>21</v>
       </c>
@@ -633,12 +633,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -649,7 +649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>

</xml_diff>